<commit_message>
created Requirement and StudnetTerm. Updated Doc
</commit_message>
<xml_diff>
--- a/Docs/DegreePlannerDataSampleNew.xlsx
+++ b/Docs/DegreePlannerDataSampleNew.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531439\Desktop\DegreePlanner\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charan\Desktop\DOTNET_PROJECT\DegreePlanner\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5630027-6461-4F58-B903-92F19011345D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="DegreePlan" sheetId="5" r:id="rId6"/>
     <sheet name="Student" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -45,9 +44,6 @@
   </si>
   <si>
     <t>RequirementID</t>
-  </si>
-  <si>
-    <t>Requirement(unique,max 6)</t>
   </si>
   <si>
     <t>RequirementName(unique, max 20)</t>
@@ -188,9 +184,6 @@
     <t>TermAbbrev</t>
   </si>
   <si>
-    <t>Term Label</t>
-  </si>
-  <si>
     <t>S19</t>
   </si>
   <si>
@@ -316,11 +309,17 @@
   <si>
     <t>DegreePlanAbbrev(u,8)</t>
   </si>
+  <si>
+    <t>TermLabel</t>
+  </si>
+  <si>
+    <t>RequirementAbbrev(unique,max 6)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -686,7 +685,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -709,19 +708,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -749,16 +748,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
         <v>89</v>
-      </c>
-      <c r="E2" t="s">
-        <v>91</v>
       </c>
       <c r="F2" t="str">
         <f>D2&amp;A1&amp;"="&amp;A2&amp;", "&amp;B1&amp;"= '"&amp;B2&amp;"', "&amp;C1&amp;"= '"&amp;C2&amp;"'"&amp;E2</f>
@@ -1752,11 +1751,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1772,10 +1771,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D1" s="1"/>
     </row>
@@ -1784,10 +1783,10 @@
         <v>460</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1795,10 +1794,10 @@
         <v>356</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1806,10 +1805,10 @@
         <v>542</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1817,10 +1816,10 @@
         <v>563</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1828,10 +1827,10 @@
         <v>560</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1839,10 +1838,10 @@
         <v>555</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1850,10 +1849,10 @@
         <v>618</v>
       </c>
       <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1861,10 +1860,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1872,10 +1871,10 @@
         <v>664</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1883,10 +1882,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1894,10 +1893,10 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1905,10 +1904,10 @@
         <v>691</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1916,10 +1915,10 @@
         <v>692</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2909,7 +2908,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4421,11 +4420,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="157" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A8" zoomScale="157" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4439,19 +4438,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4465,10 +4464,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4482,10 +4481,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4499,10 +4498,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -4516,10 +4515,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -4533,10 +4532,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -4550,10 +4549,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -4567,10 +4566,10 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -4584,10 +4583,10 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -4601,10 +4600,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -4618,10 +4617,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -4635,10 +4634,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -4652,10 +4651,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -4669,10 +4668,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -4686,10 +4685,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -4703,10 +4702,10 @@
         <v>5</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -4720,10 +4719,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -4737,10 +4736,10 @@
         <v>2</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -4754,10 +4753,10 @@
         <v>3</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -4771,10 +4770,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4788,10 +4787,10 @@
         <v>5</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5780,7 +5779,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5798,13 +5797,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -8064,10 +8063,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+    <sheetView zoomScale="116" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -8082,19 +8081,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8108,10 +8107,10 @@
         <v>531519</v>
       </c>
       <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
         <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -8125,10 +8124,10 @@
         <v>531519</v>
       </c>
       <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
         <v>42</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -8142,10 +8141,10 @@
         <v>531499</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
         <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -8159,10 +8158,10 @@
         <v>531499</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
         <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -8176,10 +8175,10 @@
         <v>531370</v>
       </c>
       <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
         <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -8193,10 +8192,10 @@
         <v>531370</v>
       </c>
       <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
         <v>42</v>
-      </c>
-      <c r="E7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -8210,10 +8209,10 @@
         <v>531439</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
         <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -8227,10 +8226,10 @@
         <v>531439</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
         <v>42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9220,7 +9219,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9239,16 +9238,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="E1" s="1">
         <v>919</v>
@@ -9259,13 +9258,13 @@
         <v>531519</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2">
         <v>919562791</v>
@@ -9276,13 +9275,13 @@
         <v>531499</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="5">
         <v>919558726</v>
@@ -9293,13 +9292,13 @@
         <v>531370</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="5">
         <v>919563101</v>
@@ -9310,13 +9309,13 @@
         <v>531439</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="5">
         <v>919563365</v>

</xml_diff>